<commit_message>
add the test cases
</commit_message>
<xml_diff>
--- a/jobs/1AI_test_try/output/summary.xlsx
+++ b/jobs/1AI_test_try/output/summary.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>test2</t>
+          <t>test1</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -458,7 +458,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>test1</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="B3" t="n">

</xml_diff>